<commit_message>
Access Key used from QA.properties
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\automation-work\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\automation-framework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D5E6AA-E3F0-49C0-B37B-9FE87CBF3B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D18430C-373C-44D7-BBCF-170A3855C759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="850" windowWidth="7610" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -392,9 +392,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{FA196535-5782-434F-9DFC-0C6099A19387}"/>

</xml_diff>